<commit_message>
updating the final paper
</commit_message>
<xml_diff>
--- a/Data/Data Dictionary.xlsx
+++ b/Data/Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew's Surface\Documents\ETL_Group_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{030EAC5A-1F52-4760-813B-4327EA9102DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E3FF10-EC83-44DB-9A64-9E4875684226}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{E8B3E737-90B6-4ADD-903D-F87F5514B960}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
   <si>
     <t>Field Name</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Dentist</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
   </si>
 </sst>
 </file>
@@ -280,6 +283,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -289,10 +296,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90292A87-AC20-45AB-963C-785784BA1281}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="126" workbookViewId="0">
+      <selection sqref="A1:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -624,14 +627,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
@@ -657,7 +660,7 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -681,7 +684,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D4" s="2">
         <v>30</v>
@@ -701,7 +704,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D5" s="2">
         <v>30</v>
@@ -717,7 +720,7 @@
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -737,7 +740,7 @@
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -777,7 +780,7 @@
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -801,7 +804,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2">
         <v>30</v>
@@ -857,7 +860,7 @@
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -877,7 +880,7 @@
       <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -901,7 +904,7 @@
         <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D15" s="2">
         <v>30</v>
@@ -933,13 +936,13 @@
         <v>34</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" s="12" t="s">
+      <c r="A18" s="9" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new table to data dictionary
</commit_message>
<xml_diff>
--- a/Data/Data Dictionary.xlsx
+++ b/Data/Data Dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew's Surface\Documents\ETL_Group_Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbigg\Desktop\Data_Analytics\Group_Project_2\ETL_project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E3FF10-EC83-44DB-9A64-9E4875684226}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F4C0B2-A9E0-43F8-A90A-22738663E923}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{E8B3E737-90B6-4ADD-903D-F87F5514B960}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E8B3E737-90B6-4ADD-903D-F87F5514B960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="64">
   <si>
     <t>Field Name</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Sample</t>
   </si>
   <si>
-    <t>drug_info</t>
-  </si>
-  <si>
     <t>drug_id</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>This is the unique ID for a particular opioid</t>
   </si>
   <si>
-    <t>CHAR</t>
-  </si>
-  <si>
     <t>This is the drug name</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>This is the death count by opioids</t>
   </si>
   <si>
-    <t>state_info</t>
-  </si>
-  <si>
     <t>state_name</t>
   </si>
   <si>
@@ -116,12 +107,6 @@
     <t>This is the population of the state</t>
   </si>
   <si>
-    <t>dr_info</t>
-  </si>
-  <si>
-    <t>dr_id</t>
-  </si>
-  <si>
     <t>state_id</t>
   </si>
   <si>
@@ -134,9 +119,6 @@
     <t>This denotes the gender of the DR</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>This denotes the unique ID of the dr</t>
   </si>
   <si>
@@ -152,10 +134,94 @@
     <t>foreign key</t>
   </si>
   <si>
-    <t>Dentist</t>
-  </si>
-  <si>
     <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>opioids</t>
+  </si>
+  <si>
+    <t>states</t>
+  </si>
+  <si>
+    <t>state_abbv</t>
+  </si>
+  <si>
+    <t>This is the state abbreviation</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>prescribers</t>
+  </si>
+  <si>
+    <t>doctor_id</t>
+  </si>
+  <si>
+    <t>KEY</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>M.D.</t>
+  </si>
+  <si>
+    <t>prescriptions</t>
+  </si>
+  <si>
+    <t>ACETAMINOPHEN_CODEINE</t>
+  </si>
+  <si>
+    <t>DIPHENOXYLATE_ATROPINE</t>
+  </si>
+  <si>
+    <t>FENTANYL</t>
+  </si>
+  <si>
+    <t>HYDROCODONE_ACETAMINOPHEN</t>
+  </si>
+  <si>
+    <t>HYDROMORPHONE_HCL</t>
+  </si>
+  <si>
+    <t>METHADONE_HCL</t>
+  </si>
+  <si>
+    <t>MORPHINE_SULFATE</t>
+  </si>
+  <si>
+    <t>OXYCODONE_ACETAMINOPHEN</t>
+  </si>
+  <si>
+    <t>OXYCODONE_HCL</t>
+  </si>
+  <si>
+    <t>OXYCONTIN</t>
+  </si>
+  <si>
+    <t>TRAMADOL_HCL</t>
+  </si>
+  <si>
+    <t>Total_Opioid_Prescriptions</t>
+  </si>
+  <si>
+    <t>Opioid_Prescriber</t>
+  </si>
+  <si>
+    <t>MORPHINE_SULFATE_ER</t>
+  </si>
+  <si>
+    <t>This is the number of prescriptions of this drug</t>
+  </si>
+  <si>
+    <t>Total number of opioid prescriptions per physician</t>
+  </si>
+  <si>
+    <t>If physician has prescribed opioids</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -267,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -283,9 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -294,6 +358,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -610,33 +681,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90292A87-AC20-45AB-963C-785784BA1281}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" workbookViewId="0">
-      <selection sqref="A1:F18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.90625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="13"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -655,295 +730,591 @@
       <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G2" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2">
         <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="6">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G3" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2">
         <v>30</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2">
         <v>30</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>7</v>
+      <c r="B6" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2">
         <v>4</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="6">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>30</v>
+        <v>15</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2">
         <v>100000</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F8" s="6">
         <v>13543</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2">
         <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2">
+        <v>30</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2">
+        <v>10000000000</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="6">
+        <v>8623000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1780937842</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2">
+        <v>100</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2">
         <v>10</v>
       </c>
-      <c r="D11" s="2">
-        <v>10000000000</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="6">
-        <v>8623000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="F17" s="6">
+        <v>1780937842</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="12">
+        <v>5</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="12">
+        <v>5</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="12">
+        <v>5</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="12">
+        <v>5</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="12">
+        <v>5</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="12">
+        <v>5</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="12">
+        <v>5</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="12">
+        <v>5</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="12">
+        <v>5</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="12">
+        <v>5</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="12">
+        <v>5</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="12">
+        <v>5</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="12">
         <v>10</v>
       </c>
-      <c r="D12" s="2">
-        <v>10</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="6">
-        <v>1780937842</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="2">
-        <v>2</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="2">
-        <v>4</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="2">
-        <v>30</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="2">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="6" t="s">
+      <c r="E30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="13">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" s="9" t="s">
-        <v>39</v>
+      <c r="D31" s="12">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>